<commit_message>
Agregando SKU a articulos para mejorar busqueda
</commit_message>
<xml_diff>
--- a/Consultas externas Mis Consultas Externas Emporio Lista Minorista ConIVA y Proveedor.xlsx
+++ b/Consultas externas Mis Consultas Externas Emporio Lista Minorista ConIVA y Proveedor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tango\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tango\Desktop\Tienda Web\startbootstrap-shop-homepage-gh-pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA33079D-6A1E-4B80-8540-C4A1BF0C7B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4902D0FE-EFEA-48CE-BC10-111209275F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="2925" windowWidth="10830" windowHeight="7875" xr2:uid="{8E8B65D7-B3E5-42CB-8A3E-B8F139F1F4DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8E8B65D7-B3E5-42CB-8A3E-B8F139F1F4DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista Minorista ConIVA y Provee" sheetId="1" r:id="rId1"/>
@@ -9446,7 +9446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C6B4CC-6E7C-47FC-9CE6-B02295EBE3CD}">
   <dimension ref="A1:F1431"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>